<commit_message>
Debug of Class Quench Detection, Application of effective insulation area function
</commit_message>
<xml_diff>
--- a/test/quench_detection/illustration_sheet_quench_detection.xlsx
+++ b/test/quench_detection/illustration_sheet_quench_detection.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9645" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="geometry" sheetId="3" r:id="rId1"/>
@@ -1877,7 +1877,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1995,7 +1994,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4856,7 +4854,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4974,7 +4971,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -9424,15 +9420,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
+      <xdr:colOff>9525</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>28574</xdr:rowOff>
+      <xdr:rowOff>9524</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>590551</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -11344,8 +11340,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I102"/>
   <sheetViews>
-    <sheetView topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="Q24" sqref="Q24:R24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19642,8 +19638,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O31" sqref="O31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>